<commit_message>
Test Case Failed case implmented
</commit_message>
<xml_diff>
--- a/Data/TestData/EmployeeData.xlsx
+++ b/Data/TestData/EmployeeData.xlsx
@@ -433,9 +433,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -489,13 +489,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -507,6 +500,13 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -558,6 +558,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -566,22 +582,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -681,6 +681,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -712,18 +724,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,6 +851,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -881,26 +901,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -927,22 +927,22 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -951,7 +951,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -963,25 +963,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -996,19 +996,19 @@
     <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1017,55 +1017,55 @@
     <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1086,8 +1086,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1409,8 +1409,8 @@
   <sheetPr/>
   <dimension ref="A1:BA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BA2" sqref="BA2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -1707,16 +1707,16 @@
       <c r="AA2">
         <v>3</v>
       </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AC2" s="9" t="s">
         <v>70</v>
       </c>
       <c r="AD2" t="s">
         <v>71</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="AE2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AF2" s="14" t="s">
+      <c r="AF2" s="13" t="s">
         <v>73</v>
       </c>
       <c r="AG2" t="s">
@@ -1859,16 +1859,16 @@
       <c r="AA3">
         <v>2</v>
       </c>
-      <c r="AC3" s="13" t="s">
+      <c r="AC3" s="14" t="s">
         <v>90</v>
       </c>
       <c r="AD3" t="s">
         <v>91</v>
       </c>
-      <c r="AE3" s="14" t="s">
+      <c r="AE3" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AF3" s="13" t="s">
         <v>73</v>
       </c>
       <c r="AG3" t="s">
@@ -2008,10 +2008,10 @@
       <c r="AD4" t="s">
         <v>102</v>
       </c>
-      <c r="AE4" s="14" t="s">
+      <c r="AE4" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AF4" s="14" t="s">
+      <c r="AF4" s="13" t="s">
         <v>73</v>
       </c>
       <c r="AG4" t="s">

</xml_diff>